<commit_message>
vipe_coded most of .py files
</commit_message>
<xml_diff>
--- a/00_files_directories_naming.xlsx
+++ b/00_files_directories_naming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr-MSI\Documentos\GitHub\spacer-hb-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5420ED65-10A5-4183-B47B-D2214470237F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695B514E-2722-4957-AEFF-6E7019C4A496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1B48F93-7407-4BBB-8927-FD6BF804E657}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>PATH</t>
   </si>
@@ -41,9 +41,6 @@
     <t>BASE_DIR</t>
   </si>
   <si>
-    <t>to_github_bilbao_otxarkoaga</t>
-  </si>
-  <si>
     <t>otxarkoaga_lidar_cliped.las</t>
   </si>
   <si>
@@ -84,6 +81,15 @@
   </si>
   <si>
     <t>heat_res_curr_density_clip.tif</t>
+  </si>
+  <si>
+    <t>LOC_LONGDITUDE</t>
+  </si>
+  <si>
+    <t>LOC_LATITUDE</t>
+  </si>
+  <si>
+    <t>spacer-hb-framework</t>
   </si>
 </sst>
 </file>
@@ -474,7 +480,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,10 +491,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -501,55 +507,71 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>-2.8977909999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>43.257928</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>